<commit_message>
Finalisation de la planification initiale du projet
</commit_message>
<xml_diff>
--- a/Documentation/2023.05.02_Nonnenmacher_Enzo_Journal de travail.xlsx
+++ b/Documentation/2023.05.02_Nonnenmacher_Enzo_Journal de travail.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TPI\TPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Jour</t>
   </si>
@@ -58,6 +58,27 @@
   </si>
   <si>
     <t xml:space="preserve">Création du dépôt github </t>
+  </si>
+  <si>
+    <t>Rédaction de la planification initiale</t>
+  </si>
+  <si>
+    <t>Rédaction du rapport de projet</t>
+  </si>
+  <si>
+    <t>Rédaction de la partie "Analyse préliminaire"</t>
+  </si>
+  <si>
+    <t>Création des différents sprint sur Icescrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification de la planification initiale </t>
+  </si>
+  <si>
+    <t>J'ai rencontré pas mal de difficulté pour estimé le nombre d'heure de chaque bloc de la planification initiale</t>
+  </si>
+  <si>
+    <t>Modification de la partie Introduction du rapport</t>
   </si>
 </sst>
 </file>
@@ -152,18 +173,6 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
     </dxf>
     <dxf>
@@ -178,7 +187,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -220,13 +241,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:F7"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Jour" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="2" name="Semaine" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="3" name="Temps [h]" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="4" name="Type" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Jour" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" name="Semaine" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" name="Temps [h]" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="4" name="Type" dataDxfId="4" totalsRowDxfId="3"/>
     <tableColumn id="5" name="Description"/>
     <tableColumn id="6" name="Commentaire/Remarque"/>
   </tableColumns>
@@ -238,8 +259,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B3" totalsRowCount="1">
   <autoFilter ref="A1:B2"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="4">
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" totalsRowDxfId="0">
+      <calculatedColumnFormula>SUM(Tableau1[Temps '[h']])</calculatedColumnFormula>
       <totalsRowFormula>SUM(B2:B2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -510,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +575,9 @@
       <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="D2" s="8" t="s">
         <v>9</v>
       </c>
@@ -562,28 +586,98 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="8"/>
+      <c r="A4" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8"/>
+      <c r="A5" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8"/>
+      <c r="A6" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>45048</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -599,7 +693,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,6 +714,10 @@
       <c r="A2" s="6">
         <v>45048</v>
       </c>
+      <c r="B2" s="5">
+        <f>SUM(Tableau1[Temps '[h']])</f>
+        <v>0.20833333333333331</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -627,7 +725,7 @@
       </c>
       <c r="B3" s="12">
         <f>SUM(B2:B2)</f>
-        <v>0</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>